<commit_message>
HP: fixing: new dirList and fileList for each testcase
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students_U1.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students_U1.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="MainInfo" sheetId="3" r:id="rId1"/>
-    <sheet name="ZipFiles_U1_sub1" sheetId="4" r:id="rId2"/>
-    <sheet name="Results_U1_sub1" sheetId="5" r:id="rId3"/>
-    <sheet name="ZipFiles_U1_sub2" sheetId="1" r:id="rId4"/>
-    <sheet name="Results_U1_sub2" sheetId="2" r:id="rId5"/>
+    <sheet name="ZipFiles_U1E1_1_sub1" sheetId="4" r:id="rId2"/>
+    <sheet name="Results_U1E1_1_sub1" sheetId="5" r:id="rId3"/>
+    <sheet name="ZipFiles_U1E2_1_sub1" sheetId="1" r:id="rId4"/>
+    <sheet name="Results_U1E2_1_sub1" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="78">
   <si>
     <t>item2</t>
   </si>
@@ -35,18 +35,6 @@
     <t>item6</t>
   </si>
   <si>
-    <t>RoundU1_sub2_100000.zip</t>
-  </si>
-  <si>
-    <t>RoundU1_sub2_100001.zip</t>
-  </si>
-  <si>
-    <t>RoundU1_sub2_100002.zip</t>
-  </si>
-  <si>
-    <t>RoundU1_sub2_100003.zip</t>
-  </si>
-  <si>
     <t>Submit Zip</t>
   </si>
   <si>
@@ -146,9 +134,6 @@
     <t>sub1</t>
   </si>
   <si>
-    <t>NOTE: old file name pattern used</t>
-  </si>
-  <si>
     <t>TASKFLOW 1</t>
   </si>
   <si>
@@ -203,16 +188,10 @@
     <t>data/taskflow/taskflow3_U1E1_1_sub1.xml</t>
   </si>
   <si>
-    <t>ZipFiles_U1_sub1</t>
-  </si>
-  <si>
     <t>data/zips/Round_U1_tests/</t>
   </si>
   <si>
     <t>Round_U1_sub1_reference.zip</t>
-  </si>
-  <si>
-    <t>Results_U1_sub1</t>
   </si>
   <si>
     <t>RESULT(1) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
@@ -242,6 +221,48 @@
   </si>
   <si>
     <t>RESULT(4) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>Results_U1E2_1_sub1</t>
+  </si>
+  <si>
+    <t>ZipFiles_U1E2_1_sub1</t>
+  </si>
+  <si>
+    <t>ZipFiles_U1E1_1_sub1</t>
+  </si>
+  <si>
+    <t>Results_U1E1_1_sub1</t>
+  </si>
+  <si>
+    <t>data/taskflow/taskflow3_U1E2_1_sub1.xml</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
 )</t>
   </si>
 </sst>
@@ -249,6 +270,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -634,175 +656,224 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="45.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C2" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C5" t="str">
         <f>TEXT($C$2*10,"0")</f>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C6" t="str">
         <f>TEXT($C$2*10 + 8,"0")</f>
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="6" t="str">
-        <f>TEXT(ZipFiles_U1_sub1!E9,"0")</f>
+        <f>TEXT(ZipFiles_U1E1_1_sub1!E9,"0")</f>
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C23" s="6" t="str">
+        <f>TEXT(ZipFiles_U1E2_1_sub1!E9,"0")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="C23" s="6"/>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -816,38 +887,38 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="29.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" width="29.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -858,19 +929,19 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -887,7 +958,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -904,7 +975,7 @@
         <v>100001</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -918,7 +989,7 @@
         <v>100002</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -932,7 +1003,7 @@
         <v>100003</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -944,117 +1015,117 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A9:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="37.88671875" customWidth="1"/>
+    <col min="7" max="7" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="37.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="H11" s="3"/>
       <c r="L11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H12" s="3"/>
       <c r="L12" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="L13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="G14" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1067,35 +1138,35 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1106,19 +1177,19 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1135,7 +1206,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1152,7 +1223,7 @@
         <v>100001</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1169,7 +1240,7 @@
         <v>100002</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1186,7 +1257,7 @@
         <v>100003</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1198,108 +1269,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T14"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:AA14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="60.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="68.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="58.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.44140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.33203125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="26.5546875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="24" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="60.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="68.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="58.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="8.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="26.5546875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="24.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" t="s">
+        <v>72</v>
+      </c>
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" t="s">
+        <v>59</v>
+      </c>
+      <c r="M13" t="s">
+        <v>72</v>
+      </c>
       <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G14" s="3"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="G14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" t="s">
+        <v>77</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>

</xml_diff>

<commit_message>
HP: clearing channels at the beginning of each testcase
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students_U1.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students_U1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="106">
   <si>
     <t>item2</t>
   </si>
@@ -83,18 +83,6 @@
     <t>Testcase4</t>
   </si>
   <si>
-    <t>Errors TC1</t>
-  </si>
-  <si>
-    <t>Errors TC2</t>
-  </si>
-  <si>
-    <t>Errors TC3</t>
-  </si>
-  <si>
-    <t>Errors TC4</t>
-  </si>
-  <si>
     <t>MainInfo</t>
   </si>
   <si>
@@ -201,11 +189,163 @@
     <t>100</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>Results_U1E2_1_sub1</t>
+  </si>
+  <si>
+    <t>ZipFiles_U1E2_1_sub1</t>
+  </si>
+  <si>
+    <t>ZipFiles_U1E1_1_sub1</t>
+  </si>
+  <si>
+    <t>Results_U1E1_1_sub1</t>
+  </si>
+  <si>
+    <t>data/taskflow/taskflow3_U1E2_1_sub1.xml</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(4)  FLOW(true) MSG(TESTCASE(4):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(5)  FLOW(true) MSG(TESTCASE(5):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(6)  FLOW(true) MSG(TESTCASE(6):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(4)  FLOW(false) MSG(TESTCASE(4):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(5)  FLOW(false) MSG(TESTCASE(5):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(6)  FLOW(false) MSG(TESTCASE(6):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(2) TESTCASE(4) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-complex-type.4: Attribute 'type' must appear on element 'conveyor'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(2) TESTCASE(5) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-complex-type.4: Attribute 'modID' must appear on element 'lift_module'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(2) TESTCASE(6) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-complex-type.4: Attribute 'modID' must appear on element 'lift_module'.)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(4)  FLOW(true) MSG(TESTCASE(4):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(5)  FLOW(false) MSG(TESTCASE(5):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(6)  FLOW(false) MSG(TESTCASE(6):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(5) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-complex-type.4: Attribute 'modID' must appear on element 'lift_module'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(6) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-complex-type.4: Attribute 'modID' must appear on element 'lift_module'.)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(4)  FLOW(true) MSG(TESTCASE(4):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(5)  FLOW(true) MSG(TESTCASE(5):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(6)  FLOW(false) MSG(TESTCASE(6):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(4) TESTCASE(6) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-complex-type.2.4.b: The content of element 'conveyor' is not complete. One of '{description}' is expected.)</t>
+  </si>
+  <si>
+    <t>Points TC5</t>
+  </si>
+  <si>
+    <t>Points TC6</t>
+  </si>
+  <si>
+    <t>Testcase5</t>
+  </si>
+  <si>
+    <t>Testcase6</t>
+  </si>
+  <si>
     <t>RESULT(2) TCASE(1)  FLOW(false) MSG(TESTCASE(1):NOT-COMPARED
 )</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>ERROR: SUBMIT(2) TESTCASE(1) MSG:(CLASS:siima.app.operator.XMLWellFormedCheck ERROR:ParseError at [row,col]:[15,13]
@@ -220,50 +360,10 @@
 Message: The element type "artist" must be terminated by the matching end-tag "&lt;/artist&gt;".)</t>
   </si>
   <si>
-    <t>RESULT(4) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
-)</t>
-  </si>
-  <si>
-    <t>Results_U1E2_1_sub1</t>
-  </si>
-  <si>
-    <t>ZipFiles_U1E2_1_sub1</t>
-  </si>
-  <si>
-    <t>ZipFiles_U1E1_1_sub1</t>
-  </si>
-  <si>
-    <t>Results_U1E1_1_sub1</t>
-  </si>
-  <si>
-    <t>data/taskflow/taskflow3_U1E2_1_sub1.xml</t>
-  </si>
-  <si>
-    <t>RESULT(1) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
-)</t>
+    <t>Errors</t>
   </si>
   <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>RESULT(2) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(2) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(3) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(3) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(4) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
-)</t>
   </si>
 </sst>
 </file>
@@ -330,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -348,6 +448,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,7 +762,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,12 +774,12 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" s="7">
         <v>2</v>
@@ -681,20 +787,20 @@
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" t="str">
         <f>TEXT($C$2*10,"0")</f>
@@ -703,7 +809,7 @@
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C6" t="str">
         <f>TEXT($C$2*10 + 8,"0")</f>
@@ -712,36 +818,36 @@
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C13" s="6" t="str">
         <f>TEXT(ZipFiles_U1E1_1_sub1!E9,"0")</f>
@@ -750,68 +856,68 @@
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C23" s="6" t="str">
         <f>TEXT(ZipFiles_U1E2_1_sub1!E9,"0")</f>
@@ -820,60 +926,60 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -905,20 +1011,20 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -958,7 +1064,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -975,7 +1081,7 @@
         <v>100001</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -989,7 +1095,7 @@
         <v>100002</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1003,7 +1109,7 @@
         <v>100003</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1013,25 +1119,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A9:T14"/>
+  <dimension ref="A9:AK14"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" customWidth="true" width="18.33203125" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="20.6640625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="37.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="12.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1062,70 +1168,99 @@
       <c r="J10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="L10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
       <c r="Q10" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="L11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="Q11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="L12" t="s">
-        <v>61</v>
-      </c>
       <c r="Q12" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L13" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="G14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L14" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1161,12 +1296,12 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1206,7 +1341,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1223,7 +1358,7 @@
         <v>100001</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1240,7 +1375,7 @@
         <v>100002</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1257,7 +1392,7 @@
         <v>100003</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1267,38 +1402,43 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T14"/>
+  <dimension ref="A2:AH15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="60.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="68.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="58.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="37.109375" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="29.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.5546875" collapsed="true"/>
     <col min="13" max="13" customWidth="true" width="8.88671875" collapsed="true"/>
     <col min="14" max="14" customWidth="true" width="10.44140625" collapsed="true"/>
     <col min="15" max="15" customWidth="true" width="9.33203125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="26.5546875" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="26.88671875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="29.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1329,92 +1469,251 @@
       <c r="J10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="L10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
       <c r="Q10" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH10" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="G11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="U11" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M11" t="s">
+      <c r="V11" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G12" s="3" t="s">
+      <c r="W11" s="5"/>
+    </row>
+    <row r="12" spans="1:34" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L12" t="s">
-        <v>59</v>
-      </c>
-      <c r="M12" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q12" s="4"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G13" s="3" t="s">
+      <c r="I12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L13" t="s">
-        <v>59</v>
-      </c>
-      <c r="M13" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q13" s="3"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="K12" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="L12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="U12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="V12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="W12" s="5"/>
+      <c r="AA12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+    </row>
+    <row r="13" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q13" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="T13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="U13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="W13" s="5"/>
+      <c r="AA13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+    </row>
+    <row r="14" spans="1:34" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="G14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="L14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="Q14" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="T14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="U14" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="W14" s="5"/>
+      <c r="AA14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="L15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
HP: taskflow for U1E3_1
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students_U1.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students_U1.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="MainInfo" sheetId="3" r:id="rId1"/>
-    <sheet name="ZipFiles_U1E1_1_sub1" sheetId="4" r:id="rId2"/>
+    <sheet name="ZipFiles_U1_sub1" sheetId="4" r:id="rId2"/>
     <sheet name="Results_U1E1_1_sub1" sheetId="5" r:id="rId3"/>
-    <sheet name="ZipFiles_U1E2_1_sub1" sheetId="1" r:id="rId4"/>
-    <sheet name="Results_U1E2_1_sub1" sheetId="2" r:id="rId5"/>
+    <sheet name="Results_U1E2_1_sub1" sheetId="2" r:id="rId4"/>
+    <sheet name="Results_U1E3_1_sub1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="111">
   <si>
     <t>item2</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Round:</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>Student Submits</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>Round_U1_sub1_100003.zip</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>data/taskflow/taskflow3_U1E1_1_sub1.xml</t>
   </si>
   <si>
@@ -197,12 +191,6 @@
   </si>
   <si>
     <t>Results_U1E2_1_sub1</t>
-  </si>
-  <si>
-    <t>ZipFiles_U1E2_1_sub1</t>
-  </si>
-  <si>
-    <t>ZipFiles_U1E1_1_sub1</t>
   </si>
   <si>
     <t>Results_U1E1_1_sub1</t>
@@ -364,6 +352,45 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>ZipFiles_U1_sub1</t>
+  </si>
+  <si>
+    <t>data/taskflow/taskflow3_U1E3_1_sub1.xml</t>
+  </si>
+  <si>
+    <t>Results_U1E3_1_sub1</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(3)  FLOW(true) MSG(TESTCASE(3):NOT-EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(3) MSG:(TEXT COMPARE:DEL:(01_x000D_
+02_x000D_
+03_x000D_
+04_x000D_
+05))</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(4)  FLOW(true) MSG(TESTCASE(4):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(5)  FLOW(true) MSG(TESTCASE(5):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(5)  FLOW(true) MSG(TESTCASE(5):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(3) MSG:(TEXT COMPARE:DEL:(01
+02
+03
+04
+05))</t>
   </si>
 </sst>
 </file>
@@ -761,7 +788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -774,212 +801,269 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="str">
         <f>TEXT($C$2*10,"0")</f>
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="str">
         <f>TEXT($C$2*10 + 8,"0")</f>
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="6" t="str">
-        <f>TEXT(ZipFiles_U1E1_1_sub1!E9,"0")</f>
+        <f>TEXT(ZipFiles_U1_sub1!$E$9,"0")</f>
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="6" t="str">
-        <f>TEXT(ZipFiles_U1E2_1_sub1!E9,"0")</f>
+        <f>TEXT(ZipFiles_U1_sub1!$E$9,"0")</f>
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="2" t="s">
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
         <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="6" t="str">
+        <f>TEXT(ZipFiles_U1_sub1!$E$9,"0")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -993,7 +1077,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A12" sqref="A12:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1003,7 +1087,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1011,20 +1095,20 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1064,7 +1148,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1081,10 +1165,13 @@
         <v>100001</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1095,10 +1182,13 @@
         <v>100002</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1109,7 +1199,7 @@
         <v>100003</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1224,7 @@
   <sheetData>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -1151,71 +1241,71 @@
         <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="K10" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="Q10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="T10" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="U10" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
@@ -1225,42 +1315,42 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H11" s="3"/>
       <c r="Q11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H12" s="3"/>
       <c r="Q12" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AA12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AA13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="G14" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Q14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1270,142 +1360,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="24.109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E9" s="5">
-        <f>COUNTA(E11:E100)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>100000</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>100001</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1">
-        <v>100002</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="1">
-        <v>100003</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AH15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AA12" sqref="AA12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:AH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,12 +1388,12 @@
   <sheetData>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
@@ -1452,165 +1410,165 @@
         <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="K10" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="T10" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="U10" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="129.6" x14ac:dyDescent="0.3">
       <c r="G11" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="Q11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="R11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="S11" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="T11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="U11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="Q11" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="R11" s="9" t="s">
+      <c r="V11" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="S11" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="T11" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="U11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="V11" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="W11" s="5"/>
     </row>
     <row r="12" spans="1:34" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="Q12" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="S12" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="T12" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V12" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="W12" s="5"/>
       <c r="AA12" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AB12" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
@@ -1618,94 +1576,94 @@
     </row>
     <row r="13" spans="1:34" ht="158.4" x14ac:dyDescent="0.3">
       <c r="G13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="Q13" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="R13" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="T13" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="U13" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V13" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="W13" s="5"/>
       <c r="AA13" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="AB13" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
     </row>
-    <row r="14" spans="1:34" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G14" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="Q14" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="S14" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="T14" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="U14" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="V14" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="W14" s="5"/>
       <c r="AA14" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
@@ -1718,4 +1676,243 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A9:AH14"/>
+  <sheetViews>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH10" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>101</v>
+      </c>
+      <c r="R11" t="s">
+        <v>64</v>
+      </c>
+      <c r="S11" t="s">
+        <v>65</v>
+      </c>
+      <c r="T11" t="s">
+        <v>66</v>
+      </c>
+      <c r="U11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" t="s">
+        <v>107</v>
+      </c>
+      <c r="K12" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>101</v>
+      </c>
+      <c r="R12" t="s">
+        <v>64</v>
+      </c>
+      <c r="S12" t="s">
+        <v>65</v>
+      </c>
+      <c r="T12" t="s">
+        <v>66</v>
+      </c>
+      <c r="U12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K13" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>101</v>
+      </c>
+      <c r="R13" t="s">
+        <v>64</v>
+      </c>
+      <c r="S13" t="s">
+        <v>54</v>
+      </c>
+      <c r="T13" t="s">
+        <v>66</v>
+      </c>
+      <c r="U13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>101</v>
+      </c>
+      <c r="R14" t="s">
+        <v>64</v>
+      </c>
+      <c r="S14" t="s">
+        <v>65</v>
+      </c>
+      <c r="T14" t="s">
+        <v>66</v>
+      </c>
+      <c r="U14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>